<commit_message>
ran some stuff idk what works
</commit_message>
<xml_diff>
--- a/Plot/Cumulative_Normalized_Stats_by_DraftPos.xlsx
+++ b/Plot/Cumulative_Normalized_Stats_by_DraftPos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Desktop\MQP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Desktop\MQP\Plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BE1549-2CBC-41AF-BD7D-E6554D4B1FB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D370A3-8850-4BB3-AAFA-845F33FCF117}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5528,7 +5528,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8667023" cy="6289408"/>
+    <xdr:ext cx="8659752" cy="6289408"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5954,7 +5954,7 @@
         <v>6949900</v>
       </c>
       <c r="I2" s="3">
-        <f>SUM(G2,H2)</f>
+        <f t="shared" ref="I2:I31" si="0">SUM(G2,H2)</f>
         <v>12805100</v>
       </c>
       <c r="J2" s="5">
@@ -5981,7 +5981,7 @@
         <v>3809.677419354839</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F61" si="0">AVERAGE(C3,D3,E3)</f>
+        <f t="shared" ref="F3:F61" si="1">AVERAGE(C3,D3,E3)</f>
         <v>4111.6189442813638</v>
       </c>
       <c r="G3" s="3">
@@ -5991,7 +5991,7 @@
         <v>6218300</v>
       </c>
       <c r="I3" s="3">
-        <f>SUM(G3,H3)</f>
+        <f t="shared" si="0"/>
         <v>11457100</v>
       </c>
       <c r="J3">
@@ -6020,7 +6020,7 @@
         <v>4815.322580645161</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4693.0473892969685</v>
       </c>
       <c r="G4" s="3">
@@ -6030,7 +6030,7 @@
         <v>5584000</v>
       </c>
       <c r="I4" s="3">
-        <f>SUM(G4,H4)</f>
+        <f t="shared" si="0"/>
         <v>10288500</v>
       </c>
       <c r="J4">
@@ -6059,7 +6059,7 @@
         <v>4063.7096774193551</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4253.1548176108263</v>
       </c>
       <c r="G5" s="3">
@@ -6069,7 +6069,7 @@
         <v>5034600</v>
       </c>
       <c r="I5" s="3">
-        <f>SUM(G5,H5)</f>
+        <f t="shared" si="0"/>
         <v>9276300</v>
       </c>
       <c r="J5">
@@ -6098,7 +6098,7 @@
         <v>4803.2258064516127</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4556.2360734044642</v>
       </c>
       <c r="G6" s="3">
@@ -6108,7 +6108,7 @@
         <v>4559100</v>
       </c>
       <c r="I6" s="3">
-        <f>SUM(G6,H6)</f>
+        <f t="shared" si="0"/>
         <v>8400100</v>
       </c>
       <c r="J6">
@@ -6137,7 +6137,7 @@
         <v>1586.2903225806449</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2051.7084097123266</v>
       </c>
       <c r="G7" s="3">
@@ -6147,7 +6147,7 @@
         <v>4140900</v>
       </c>
       <c r="I7" s="3">
-        <f>SUM(G7,H7)</f>
+        <f t="shared" si="0"/>
         <v>7629500</v>
       </c>
       <c r="J7">
@@ -6176,7 +6176,7 @@
         <v>2223.3870967741932</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2869.9554877302094</v>
       </c>
       <c r="G8" s="3">
@@ -6186,7 +6186,7 @@
         <v>3780100</v>
       </c>
       <c r="I8" s="3">
-        <f>SUM(G8,H8)</f>
+        <f t="shared" si="0"/>
         <v>6964800</v>
       </c>
       <c r="J8">
@@ -6215,7 +6215,7 @@
         <v>1787.9032258064519</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2547.1050596659684</v>
       </c>
       <c r="G9" s="3">
@@ -6225,7 +6225,7 @@
         <v>3463100</v>
       </c>
       <c r="I9" s="3">
-        <f>SUM(G9,H9)</f>
+        <f t="shared" si="0"/>
         <v>6380700</v>
       </c>
       <c r="J9">
@@ -6254,7 +6254,7 @@
         <v>3504.0322580645161</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3741.366301086457</v>
       </c>
       <c r="G10" s="3">
@@ -6264,7 +6264,7 @@
         <v>3183300</v>
       </c>
       <c r="I10" s="3">
-        <f>SUM(G10,H10)</f>
+        <f t="shared" si="0"/>
         <v>5865200</v>
       </c>
       <c r="J10">
@@ -6293,7 +6293,7 @@
         <v>2795.9677419354848</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3201.6965149689509</v>
       </c>
       <c r="G11" s="3">
@@ -6303,7 +6303,7 @@
         <v>3024100</v>
       </c>
       <c r="I11" s="3">
-        <f>SUM(G11,H11)</f>
+        <f t="shared" si="0"/>
         <v>5571800</v>
       </c>
       <c r="J11">
@@ -6332,7 +6332,7 @@
         <v>1886.2903225806449</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2489.324268020403</v>
       </c>
       <c r="G12" s="3">
@@ -6342,7 +6342,7 @@
         <v>2872900</v>
       </c>
       <c r="I12" s="3">
-        <f>SUM(G12,H12)</f>
+        <f t="shared" si="0"/>
         <v>5293300</v>
       </c>
       <c r="J12">
@@ -6371,7 +6371,7 @@
         <v>841.12903225806417</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1572.5345913256551</v>
       </c>
       <c r="G13" s="3">
@@ -6381,7 +6381,7 @@
         <v>2729400</v>
       </c>
       <c r="I13" s="3">
-        <f>SUM(G13,H13)</f>
+        <f t="shared" si="0"/>
         <v>5028800</v>
       </c>
       <c r="J13">
@@ -6410,7 +6410,7 @@
         <v>2216.9354838709678</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2746.5924535023864</v>
       </c>
       <c r="G14" s="3">
@@ -6420,7 +6420,7 @@
         <v>2592900</v>
       </c>
       <c r="I14" s="3">
-        <f>SUM(G14,H14)</f>
+        <f t="shared" si="0"/>
         <v>4777300</v>
       </c>
       <c r="J14">
@@ -6449,7 +6449,7 @@
         <v>1288.7096774193551</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1776.4117470869423</v>
       </c>
       <c r="G15" s="3">
@@ -6459,7 +6459,7 @@
         <v>2463200</v>
       </c>
       <c r="I15" s="3">
-        <f>SUM(G15,H15)</f>
+        <f t="shared" si="0"/>
         <v>4538500</v>
       </c>
       <c r="J15">
@@ -6488,7 +6488,7 @@
         <v>1233.8709677419361</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1866.0711036590255</v>
       </c>
       <c r="G16" s="3">
@@ -6498,7 +6498,7 @@
         <v>2339900</v>
       </c>
       <c r="I16" s="3">
-        <f>SUM(G16,H16)</f>
+        <f t="shared" si="0"/>
         <v>4311200</v>
       </c>
       <c r="J16">
@@ -6527,7 +6527,7 @@
         <v>1071.7741935483871</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1762.7481035232502</v>
       </c>
       <c r="G17" s="3">
@@ -6537,7 +6537,7 @@
         <v>2223000</v>
       </c>
       <c r="I17" s="3">
-        <f>SUM(G17,H17)</f>
+        <f t="shared" si="0"/>
         <v>4095900</v>
       </c>
       <c r="J17">
@@ -6566,7 +6566,7 @@
         <v>1222.58064516129</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1702.5353740965609</v>
       </c>
       <c r="G18" s="3">
@@ -6576,7 +6576,7 @@
         <v>2111900</v>
       </c>
       <c r="I18" s="3">
-        <f>SUM(G18,H18)</f>
+        <f t="shared" si="0"/>
         <v>3891100</v>
       </c>
       <c r="J18">
@@ -6605,7 +6605,7 @@
         <v>1225.8064516129029</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1926.2715232029193</v>
       </c>
       <c r="G19" s="3">
@@ -6615,7 +6615,7 @@
         <v>2006300</v>
       </c>
       <c r="I19" s="3">
-        <f>SUM(G19,H19)</f>
+        <f t="shared" si="0"/>
         <v>3696600</v>
       </c>
       <c r="J19">
@@ -6644,7 +6644,7 @@
         <v>562.0967741935483</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1366.9350265516068</v>
       </c>
       <c r="G20" s="3">
@@ -6654,7 +6654,7 @@
         <v>1915900</v>
       </c>
       <c r="I20" s="3">
-        <f>SUM(G20,H20)</f>
+        <f t="shared" si="0"/>
         <v>3530000</v>
       </c>
       <c r="J20">
@@ -6683,7 +6683,7 @@
         <v>472.58064516129042</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1169.5076011361768</v>
       </c>
       <c r="G21" s="3">
@@ -6693,7 +6693,7 @@
         <v>1839200</v>
       </c>
       <c r="I21" s="3">
-        <f>SUM(G21,H21)</f>
+        <f t="shared" si="0"/>
         <v>3388700</v>
       </c>
       <c r="J21">
@@ -6722,7 +6722,7 @@
         <v>1239.516129032258</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1703.638008815519</v>
       </c>
       <c r="G22" s="3">
@@ -6732,7 +6732,7 @@
         <v>1765700</v>
       </c>
       <c r="I22" s="3">
-        <f>SUM(G22,H22)</f>
+        <f t="shared" si="0"/>
         <v>3253200</v>
       </c>
       <c r="J22">
@@ -6761,7 +6761,7 @@
         <v>630.64516129032245</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1055.6178841884448</v>
       </c>
       <c r="G23" s="3">
@@ -6771,7 +6771,7 @@
         <v>1695100</v>
       </c>
       <c r="I23" s="3">
-        <f>SUM(G23,H23)</f>
+        <f t="shared" si="0"/>
         <v>3123200</v>
       </c>
       <c r="J23">
@@ -6800,7 +6800,7 @@
         <v>650.00000000000011</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1437.0624086415773</v>
       </c>
       <c r="G24" s="3">
@@ -6810,7 +6810,7 @@
         <v>1627300</v>
       </c>
       <c r="I24" s="3">
-        <f>SUM(G24,H24)</f>
+        <f t="shared" si="0"/>
         <v>2998300</v>
       </c>
       <c r="J24">
@@ -6839,7 +6839,7 @@
         <v>1349.1935483870971</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1677.1698160874651</v>
       </c>
       <c r="G25" s="3">
@@ -6849,7 +6849,7 @@
         <v>1562200</v>
       </c>
       <c r="I25" s="3">
-        <f>SUM(G25,H25)</f>
+        <f t="shared" si="0"/>
         <v>2878400</v>
       </c>
       <c r="J25">
@@ -6878,7 +6878,7 @@
         <v>699.19354838709683</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1094.433426599843</v>
       </c>
       <c r="G26" s="3">
@@ -6888,7 +6888,7 @@
         <v>1499700</v>
       </c>
       <c r="I26" s="3">
-        <f>SUM(G26,H26)</f>
+        <f t="shared" si="0"/>
         <v>2763200</v>
       </c>
       <c r="J26">
@@ -6917,7 +6917,7 @@
         <v>969.35483870967744</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1405.7475852871751</v>
       </c>
       <c r="G27" s="3">
@@ -6927,7 +6927,7 @@
         <v>1450000</v>
       </c>
       <c r="I27" s="3">
-        <f>SUM(G27,H27)</f>
+        <f t="shared" si="0"/>
         <v>2671600</v>
       </c>
       <c r="J27">
@@ -6956,7 +6956,7 @@
         <v>647.58064516129036</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1213.3305330292467</v>
       </c>
       <c r="G28" s="3">
@@ -6966,7 +6966,7 @@
         <v>1408200</v>
       </c>
       <c r="I28" s="3">
-        <f>SUM(G28,H28)</f>
+        <f t="shared" si="0"/>
         <v>2594500</v>
       </c>
       <c r="J28">
@@ -6995,7 +6995,7 @@
         <v>324.99999999999989</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>957.37054287892931</v>
       </c>
       <c r="G29" s="3">
@@ -7005,7 +7005,7 @@
         <v>1399600</v>
       </c>
       <c r="I29" s="3">
-        <f>SUM(G29,H29)</f>
+        <f t="shared" si="0"/>
         <v>2578700</v>
       </c>
       <c r="J29">
@@ -7034,7 +7034,7 @@
         <v>320.96774193548379</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>846.00435190431745</v>
       </c>
       <c r="G30" s="3">
@@ -7044,7 +7044,7 @@
         <v>1389300</v>
       </c>
       <c r="I30" s="3">
-        <f>SUM(G30,H30)</f>
+        <f t="shared" si="0"/>
         <v>2559800</v>
       </c>
       <c r="J30">
@@ -7073,7 +7073,7 @@
         <v>604.83870967741927</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>956.85766809572272</v>
       </c>
       <c r="G31" s="3">
@@ -7083,7 +7083,7 @@
         <v>1379300</v>
       </c>
       <c r="I31" s="3">
-        <f>SUM(G31,H31)</f>
+        <f t="shared" si="0"/>
         <v>2541400</v>
       </c>
       <c r="J31">
@@ -7112,7 +7112,7 @@
         <v>408.0645161290322</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>752.55163335383725</v>
       </c>
       <c r="G32" s="3">
@@ -7150,7 +7150,7 @@
         <v>302.41935483870952</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>541.20290931481384</v>
       </c>
       <c r="G33" s="3">
@@ -7187,7 +7187,7 @@
         <v>91.129032258064498</v>
       </c>
       <c r="F34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>556.76767608149601</v>
       </c>
       <c r="G34" s="3">
@@ -7224,7 +7224,7 @@
         <v>105.64516129032251</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>512.86400068127261</v>
       </c>
       <c r="G35" s="3">
@@ -7261,7 +7261,7 @@
         <v>626.61290322580646</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>920.8097070163534</v>
       </c>
       <c r="G36" s="3">
@@ -7298,7 +7298,7 @@
         <v>172.58064516129031</v>
       </c>
       <c r="F37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>428.75066477807087</v>
       </c>
       <c r="G37" s="3">
@@ -7335,7 +7335,7 @@
         <v>206.45161290322591</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>634.43051351991414</v>
       </c>
       <c r="G38" s="3">
@@ -7372,7 +7372,7 @@
         <v>298.38709677419348</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>628.84956563984701</v>
       </c>
       <c r="G39" s="3">
@@ -7409,7 +7409,7 @@
         <v>150.8064516129032</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>505.14071583533547</v>
       </c>
       <c r="G40" s="3">
@@ -7446,7 +7446,7 @@
         <v>87.903225806451616</v>
       </c>
       <c r="F41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>502.88882202258236</v>
       </c>
       <c r="G41" s="3">
@@ -7483,7 +7483,7 @@
         <v>226.61290322580641</v>
       </c>
       <c r="F42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>456.73397208860052</v>
       </c>
       <c r="G42" s="3">
@@ -7520,7 +7520,7 @@
         <v>73.387096774193537</v>
       </c>
       <c r="F43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>364.59083858784396</v>
       </c>
       <c r="G43" s="3">
@@ -7557,7 +7557,7 @@
         <v>332.25806451612902</v>
       </c>
       <c r="F44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>682.42407588411174</v>
       </c>
       <c r="G44" s="3">
@@ -7594,7 +7594,7 @@
         <v>17.741935483870979</v>
       </c>
       <c r="F45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>321.84674970698256</v>
       </c>
       <c r="G45" s="3">
@@ -7631,7 +7631,7 @@
         <v>711.29032258064512</v>
       </c>
       <c r="F46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>898.74330415635779</v>
       </c>
       <c r="G46" s="3">
@@ -7668,7 +7668,7 @@
         <v>719.35483870967732</v>
       </c>
       <c r="F47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>845.40711945900966</v>
       </c>
       <c r="G47" s="3">
@@ -7705,7 +7705,7 @@
         <v>434.67741935483872</v>
       </c>
       <c r="F48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>763.24233699250965</v>
       </c>
       <c r="G48" s="3">
@@ -7742,7 +7742,7 @@
         <v>473.38709677419348</v>
       </c>
       <c r="F49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>578.94102729202018</v>
       </c>
       <c r="G49" s="3">
@@ -7779,7 +7779,7 @@
         <v>93.548387096774206</v>
       </c>
       <c r="F50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>287.00812527744409</v>
       </c>
       <c r="G50" s="3">
@@ -7816,7 +7816,7 @@
         <v>69.354838709677409</v>
       </c>
       <c r="F51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>339.51255705725026</v>
       </c>
       <c r="G51" s="3">
@@ -7853,7 +7853,7 @@
         <v>135.48387096774189</v>
       </c>
       <c r="F52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>228.83541981961721</v>
       </c>
       <c r="G52" s="3">
@@ -7890,7 +7890,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>224.75685927981348</v>
       </c>
       <c r="G53" s="3">
@@ -7927,7 +7927,7 @@
         <v>272.58064516129042</v>
       </c>
       <c r="F54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>431.48776999269262</v>
       </c>
       <c r="G54" s="3">
@@ -7964,7 +7964,7 @@
         <v>-16.93548387096774</v>
       </c>
       <c r="F55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>170.82806639069443</v>
       </c>
       <c r="G55" s="3">
@@ -8001,7 +8001,7 @@
         <v>101.61290322580651</v>
       </c>
       <c r="F56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>265.22627939975195</v>
       </c>
       <c r="G56" s="3">
@@ -8038,7 +8038,7 @@
         <v>137.09677419354841</v>
       </c>
       <c r="F57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>267.96312709473358</v>
       </c>
       <c r="G57" s="3">
@@ -8075,7 +8075,7 @@
         <v>29.838709677419349</v>
       </c>
       <c r="F58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65.120805127162768</v>
       </c>
       <c r="G58" s="3">
@@ -8112,7 +8112,7 @@
         <v>32.258064516129032</v>
       </c>
       <c r="F59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>98.469574098923204</v>
       </c>
       <c r="G59" s="3">
@@ -8149,7 +8149,7 @@
         <v>-16.93548387096774</v>
       </c>
       <c r="F60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.7121846838506851</v>
       </c>
       <c r="G60" s="3">
@@ -8186,7 +8186,7 @@
         <v>154.83870967741939</v>
       </c>
       <c r="F61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>190.48348602027991</v>
       </c>
       <c r="G61" s="3">

</xml_diff>